<commit_message>
update some files, add analysis file
</commit_message>
<xml_diff>
--- a/matIB2d/Examples/Example_Sawtooth/Sawtooth_Pump_Parameters.xlsx
+++ b/matIB2d/Examples/Example_Sawtooth/Sawtooth_Pump_Parameters.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/battistn/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/battistn/Desktop/IB2d/matIB2d/Examples/Example_Sawtooth/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="4660" yWindow="1920" windowWidth="28800" windowHeight="17600" tabRatio="500"/>
+    <workbookView xWindow="5240" yWindow="1060" windowWidth="28800" windowHeight="17600" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -17,22 +17,27 @@
   <definedNames>
     <definedName name="a">Sheet1!$B$17</definedName>
     <definedName name="d">Sheet1!$B$11</definedName>
+    <definedName name="d_pap">Sheet1!$G$22</definedName>
     <definedName name="ds">Sheet1!$B$9</definedName>
     <definedName name="dx">Sheet1!$B$7</definedName>
     <definedName name="dy">Sheet1!$B$8</definedName>
     <definedName name="f">Sheet1!$B$13</definedName>
     <definedName name="G">Sheet1!$B$12</definedName>
+    <definedName name="G_pap">Sheet1!$G$24</definedName>
     <definedName name="L">Sheet1!$B$16</definedName>
+    <definedName name="L_cm">Sheet1!$E$14</definedName>
+    <definedName name="L_mm">Sheet1!$E$15</definedName>
+    <definedName name="L_pap">Sheet1!$G$23</definedName>
     <definedName name="Lx">Sheet1!$B$3</definedName>
     <definedName name="Ly">Sheet1!$B$4</definedName>
-    <definedName name="mu">Sheet1!$B$19</definedName>
+    <definedName name="mu">Sheet1!$B$18</definedName>
     <definedName name="Nx">Sheet1!$B$5</definedName>
     <definedName name="Ny">Sheet1!$B$6</definedName>
     <definedName name="occ">Sheet1!$B$15</definedName>
     <definedName name="rho">Sheet1!$B$14</definedName>
     <definedName name="w">Sheet1!$B$10</definedName>
   </definedNames>
-  <calcPr calcId="150000" concurrentCalc="0"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -45,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="48">
   <si>
     <t>Lx</t>
   </si>
@@ -144,13 +149,58 @@
   </si>
   <si>
     <t>mu</t>
+  </si>
+  <si>
+    <t>NON-DIMENSIONAL RELATIONSHIPS</t>
+  </si>
+  <si>
+    <t>L_cm</t>
+  </si>
+  <si>
+    <t>L_mm</t>
+  </si>
+  <si>
+    <t>PAPER UNITS</t>
+  </si>
+  <si>
+    <t>nu</t>
+  </si>
+  <si>
+    <t>0.01 cm^2 s</t>
+  </si>
+  <si>
+    <t>PAPER RE</t>
+  </si>
+  <si>
+    <t>fa</t>
+  </si>
+  <si>
+    <t>SIMULATION RE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">nu </t>
+  </si>
+  <si>
+    <t>(kinematic visc.)</t>
+  </si>
+  <si>
+    <t>Re (old)</t>
+  </si>
+  <si>
+    <t>Re (new): faLd/G(nu)</t>
+  </si>
+  <si>
+    <t>G_pap</t>
+  </si>
+  <si>
+    <t>L_pap</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -170,6 +220,22 @@
       <b/>
       <sz val="12"/>
       <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="4" tint="-0.249977111117893"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF7030A0"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -195,12 +261,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -209,9 +278,14 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -489,32 +563,33 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E34"/>
+  <dimension ref="A1:O44"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D29" sqref="D29"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="G39" sqref="G39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="14.1640625" customWidth="1"/>
+    <col min="5" max="5" width="10.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1" s="5" t="s">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A1" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="B1" s="5"/>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" s="4" t="s">
+      <c r="B1" s="8"/>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A2" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="3" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>0</v>
       </c>
@@ -522,7 +597,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>1</v>
       </c>
@@ -537,7 +612,7 @@
         <v>26.88</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>2</v>
       </c>
@@ -545,7 +620,7 @@
         <v>512</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>3</v>
       </c>
@@ -559,7 +634,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>8</v>
       </c>
@@ -575,7 +650,7 @@
         <v>7.5410999999999992</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>10</v>
       </c>
@@ -591,7 +666,7 @@
         <v>75.410999999999987</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>4</v>
       </c>
@@ -607,7 +682,7 @@
         <v>754.1099999999999</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>5</v>
       </c>
@@ -622,7 +697,7 @@
         <v>7541.0999999999985</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
         <v>9</v>
       </c>
@@ -636,40 +711,67 @@
         <f>rho*(d)*(occ*d*f)/D11</f>
         <v>188.52749999999997</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="K11">
+        <f>1/0.01*1*d</f>
+        <v>63</v>
+      </c>
+      <c r="M11">
+        <f>1/0.01*(f*occ*B23)*B22</f>
+        <v>38.902499999999996</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B12">
-        <v>0.25</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+        <v>0.32500000000000001</v>
+      </c>
+      <c r="M12">
+        <f>f*occ*G</f>
+        <v>0.61749999999999994</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B13">
         <v>2</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D13" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
         <v>13</v>
       </c>
       <c r="B14">
         <v>1000</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D14" t="s">
+        <v>34</v>
+      </c>
+      <c r="E14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
         <v>15</v>
       </c>
       <c r="B15">
         <v>0.95</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D15" t="s">
+        <v>35</v>
+      </c>
+      <c r="E15">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
         <v>19</v>
       </c>
@@ -678,169 +780,498 @@
         <v>7.5600000000000005</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
         <v>30</v>
       </c>
       <c r="B17">
-        <f>occ*G</f>
-        <v>0.23749999999999999</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+        <v>0.33700000000000002</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
-        <v>13</v>
+        <v>32</v>
       </c>
       <c r="B18">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A19" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A20" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B20" s="4"/>
+      <c r="C20" s="4"/>
+      <c r="E20" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="F20" s="7"/>
+      <c r="G20" s="7"/>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>18</v>
+      </c>
+      <c r="B21" t="s">
+        <v>16</v>
+      </c>
+      <c r="C21" t="s">
+        <v>17</v>
+      </c>
+      <c r="E21" t="s">
+        <v>18</v>
+      </c>
+      <c r="F21" t="s">
+        <v>17</v>
+      </c>
+      <c r="G21" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A22" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B22">
+        <f>L_cm*d</f>
+        <v>0.63</v>
+      </c>
+      <c r="C22">
+        <f>L_mm*d</f>
+        <v>6.3</v>
+      </c>
+      <c r="E22" t="s">
+        <v>9</v>
+      </c>
+      <c r="F22">
+        <v>6.3</v>
+      </c>
+      <c r="G22">
+        <v>0.63</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A23" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B23">
+        <f>L_cm*G</f>
+        <v>0.32500000000000001</v>
+      </c>
+      <c r="C23">
+        <f>L_mm*G</f>
+        <v>3.25</v>
+      </c>
+      <c r="E23" t="s">
+        <v>47</v>
+      </c>
+      <c r="F23">
+        <v>76</v>
+      </c>
+      <c r="G23">
+        <v>7.6</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A24" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B24">
+        <f>L_cm*w</f>
+        <v>0.63</v>
+      </c>
+      <c r="C24">
+        <f>L_mm*w</f>
+        <v>6.3</v>
+      </c>
+      <c r="E24" t="s">
+        <v>46</v>
+      </c>
+      <c r="F24">
+        <v>3.25</v>
+      </c>
+      <c r="G24">
+        <v>0.32500000000000001</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A25" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B25">
+        <f>L_cm*L</f>
+        <v>7.5600000000000005</v>
+      </c>
+      <c r="C25">
+        <f>L_mm*L</f>
+        <v>75.600000000000009</v>
+      </c>
+      <c r="E25" t="s">
+        <v>42</v>
+      </c>
+      <c r="F25">
+        <v>1</v>
+      </c>
+      <c r="G25">
+        <v>0.01</v>
+      </c>
+      <c r="H25" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A26" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B26">
+        <f>L_cm*a</f>
+        <v>0.33700000000000002</v>
+      </c>
+      <c r="C26">
+        <f>L_mm*a</f>
+        <v>3.37</v>
+      </c>
+      <c r="E26" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="F26" s="5"/>
+      <c r="G26" s="5"/>
+      <c r="H26" s="5"/>
+      <c r="O26">
+        <f>3*7.6/0.325</f>
+        <v>70.153846153846146</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A27" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="E27" t="s">
+        <v>40</v>
+      </c>
+      <c r="F27" t="s">
+        <v>30</v>
+      </c>
+      <c r="G27" t="s">
+        <v>7</v>
+      </c>
+      <c r="H27" t="s">
+        <v>44</v>
+      </c>
+      <c r="I27" t="s">
+        <v>45</v>
+      </c>
+      <c r="J27" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A28" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="B19">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A21" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="B21" s="3"/>
-      <c r="C21" s="3"/>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
-        <v>18</v>
-      </c>
-      <c r="B22" t="s">
-        <v>16</v>
-      </c>
-      <c r="C22" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A23" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B23">
-        <f>100*d</f>
+      <c r="E28">
+        <v>1</v>
+      </c>
+      <c r="F28">
+        <v>0.33700000000000002</v>
+      </c>
+      <c r="G28">
+        <f>E28/F28</f>
+        <v>2.9673590504451037</v>
+      </c>
+      <c r="H28">
+        <f>1/0.01*E28*d</f>
         <v>63</v>
       </c>
-      <c r="C23">
-        <f>10*d</f>
-        <v>6.3</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A24" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B24">
-        <f>100*G</f>
+      <c r="I28">
+        <f>1/0.01*E28*d_pap*L_pap/G_pap</f>
+        <v>1473.2307692307691</v>
+      </c>
+      <c r="J28">
+        <f>E28*L_pap/G_pap</f>
+        <v>23.384615384615383</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="E29">
+        <v>2</v>
+      </c>
+      <c r="F29">
+        <v>0.33700000000000002</v>
+      </c>
+      <c r="G29">
+        <f t="shared" ref="G29:G30" si="0">E29/F29</f>
+        <v>5.9347181008902075</v>
+      </c>
+      <c r="H29">
+        <f>1/0.01*E29*d</f>
+        <v>126</v>
+      </c>
+      <c r="I29">
+        <f>1/0.01*E29*d_pap*L_pap/G_pap</f>
+        <v>2946.4615384615381</v>
+      </c>
+      <c r="J29">
+        <f>E29*L_pap/G_pap</f>
+        <v>46.769230769230766</v>
+      </c>
+    </row>
+    <row r="30" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A30" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="C24">
-        <f>10*G</f>
-        <v>2.5</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A25" s="2" t="s">
+      <c r="B30" s="4"/>
+      <c r="C30" s="4"/>
+      <c r="E30" s="6">
+        <v>3</v>
+      </c>
+      <c r="F30" s="6">
+        <v>0.33700000000000002</v>
+      </c>
+      <c r="G30" s="6">
+        <f t="shared" si="0"/>
+        <v>8.9020771513353107</v>
+      </c>
+      <c r="H30" s="6">
+        <f>1/0.01*E30*d</f>
+        <v>189</v>
+      </c>
+      <c r="I30" s="6">
+        <f>1/0.01*E30*d_pap*L_pap/G_pap</f>
+        <v>4419.6923076923067</v>
+      </c>
+      <c r="J30" s="6">
+        <f>E30*L_pap/G_pap</f>
+        <v>70.153846153846146</v>
+      </c>
+    </row>
+    <row r="31" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A31" s="1"/>
+      <c r="B31" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C31" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E31">
+        <v>3.5</v>
+      </c>
+      <c r="F31">
+        <v>0.33700000000000002</v>
+      </c>
+      <c r="G31">
+        <f t="shared" ref="G31" si="1">E31/F31</f>
+        <v>10.385756676557863</v>
+      </c>
+      <c r="H31">
+        <f>1/0.01*E31*d</f>
+        <v>220.5</v>
+      </c>
+      <c r="I31">
+        <f>1/0.01*E31*d_pap*L_pap/G_pap</f>
+        <v>5156.3076923076924</v>
+      </c>
+      <c r="J31">
+        <f>E31*L_pap/G_pap</f>
+        <v>81.84615384615384</v>
+      </c>
+    </row>
+    <row r="32" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>21</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C32">
+        <f>f*B26</f>
+        <v>0.67400000000000004</v>
+      </c>
+      <c r="E32">
+        <v>4</v>
+      </c>
+      <c r="F32">
+        <v>0.33700000000000002</v>
+      </c>
+      <c r="G32">
+        <f>E32/F32</f>
+        <v>11.869436201780415</v>
+      </c>
+      <c r="H32">
+        <f>1/0.01*E32*d</f>
+        <v>252</v>
+      </c>
+      <c r="I32">
+        <f>1/0.01*E32*d_pap*L_pap/G_pap</f>
+        <v>5892.9230769230762</v>
+      </c>
+      <c r="J32">
+        <f>E32*L_pap/G_pap</f>
+        <v>93.538461538461533</v>
+      </c>
+      <c r="N32">
+        <f>12/(G_pap*4)</f>
+        <v>9.2307692307692299</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>20</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C33">
+        <f>f*B26*B25/B23</f>
+        <v>15.678276923076925</v>
+      </c>
+      <c r="E33">
         <v>5</v>
       </c>
-      <c r="B25">
-        <f>100*w</f>
-        <v>63</v>
-      </c>
-      <c r="C25">
-        <f>10*w</f>
-        <v>6.3</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A26" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="B26">
-        <f>100*L</f>
-        <v>756</v>
-      </c>
-      <c r="C26">
-        <f>10*L</f>
-        <v>75.600000000000009</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A27" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="B27">
-        <f>100*a</f>
-        <v>23.75</v>
-      </c>
-      <c r="C27">
-        <f>10*a</f>
-        <v>2.375</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A28" s="2" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A29" s="2" t="s">
+      <c r="F33">
+        <v>0.33700000000000002</v>
+      </c>
+      <c r="G33">
+        <f>E33/F33</f>
+        <v>14.836795252225519</v>
+      </c>
+      <c r="H33">
+        <f>1/0.01*E33*d</f>
+        <v>315</v>
+      </c>
+      <c r="I33">
+        <f>1/0.01*E33*d_pap*L_pap/G_pap</f>
+        <v>7366.1538461538457</v>
+      </c>
+      <c r="J33">
+        <f>E33*L_pap/G_pap</f>
+        <v>116.92307692307692</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>37</v>
+      </c>
+      <c r="B34" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="C34">
+        <f>mu/rho</f>
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B37">
+        <f>10^-6*100^2</f>
+        <v>0.01</v>
+      </c>
+      <c r="E37" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="F37" s="8"/>
+      <c r="G37" s="8"/>
+      <c r="H37" s="8"/>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="E38" t="s">
+        <v>12</v>
+      </c>
+      <c r="F38" t="s">
+        <v>40</v>
+      </c>
+      <c r="G38" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A31" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="B31" s="3"/>
-      <c r="C31" s="3"/>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A32" s="1"/>
-      <c r="B32" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C32" s="4" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A33" t="s">
-        <v>21</v>
-      </c>
-      <c r="B33" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="C33">
-        <f>f*B27</f>
-        <v>47.5</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A34" t="s">
+      <c r="H38" t="s">
         <v>20</v>
       </c>
-      <c r="B34" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="C34">
-        <f>f*B27*B26/B24</f>
-        <v>1436.4</v>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="E39">
+        <v>1473.2307692307691</v>
+      </c>
+      <c r="F39">
+        <f>f*a</f>
+        <v>0.67400000000000004</v>
+      </c>
+      <c r="G39">
+        <f>(rho*F39*d*L/G)/E39</f>
+        <v>6.704526315789475</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="E40">
+        <v>2946.4615384615381</v>
+      </c>
+      <c r="F40">
+        <f>f*a</f>
+        <v>0.67400000000000004</v>
+      </c>
+      <c r="G40">
+        <f>(rho*F40*d*L/G)/E40</f>
+        <v>3.3522631578947375</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="E41" s="6">
+        <v>4419.6923076923067</v>
+      </c>
+      <c r="F41">
+        <f>f*a</f>
+        <v>0.67400000000000004</v>
+      </c>
+      <c r="G41">
+        <f>(rho*F41*d*L/G)/E41</f>
+        <v>2.2348421052631586</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="E42">
+        <v>5156.3076923076924</v>
+      </c>
+      <c r="F42">
+        <f>f*a</f>
+        <v>0.67400000000000004</v>
+      </c>
+      <c r="G42">
+        <f>(rho*F42*d*L/G)/E42</f>
+        <v>1.9155789473684213</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="E43">
+        <v>5892.9230769230762</v>
+      </c>
+      <c r="F43">
+        <f>f*a</f>
+        <v>0.67400000000000004</v>
+      </c>
+      <c r="G43">
+        <f>(rho*F43*d*L/G)/E43</f>
+        <v>1.6761315789473687</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="E44">
+        <v>7366.1538461538457</v>
+      </c>
+      <c r="F44">
+        <f>f*a</f>
+        <v>0.67400000000000004</v>
+      </c>
+      <c r="G44">
+        <f>(rho*F44*d*L/G)/E44</f>
+        <v>1.340905263157895</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="3">
-    <mergeCell ref="A21:C21"/>
+  <mergeCells count="6">
+    <mergeCell ref="E37:H37"/>
+    <mergeCell ref="A20:C20"/>
     <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A31:C31"/>
+    <mergeCell ref="A30:C30"/>
+    <mergeCell ref="E20:G20"/>
+    <mergeCell ref="E26:H26"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>